<commit_message>
Adds simulation runs and statistics as well as sanity assertions into Markov chain
</commit_message>
<xml_diff>
--- a/Probability Project Data.xlsx
+++ b/Probability Project Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oleg\Github Repositories\Python\Markov-Chain-for-Probability\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2C2DC47-C81D-4382-A2CD-B264C06324B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3752BFC9-33B2-4E57-B515-994E671BF985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4065" yWindow="4065" windowWidth="21600" windowHeight="11385" xr2:uid="{2B40AE2B-0876-AD49-A0BC-65E240822139}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="75">
   <si>
     <t>Season</t>
   </si>
@@ -208,9 +208,6 @@
   </si>
   <si>
     <t>04-05</t>
-  </si>
-  <si>
-    <t>Not Known</t>
   </si>
   <si>
     <t>03-04</t>
@@ -518,9 +515,9 @@
     <tableColumn id="30" xr3:uid="{6EB674B8-5BE9-2742-9CCD-744AFD031AEB}" name="Neutral Games Lost" dataDxfId="5"/>
     <tableColumn id="31" xr3:uid="{02DED120-2F2F-FA45-9CC5-6796E1A08117}" name="Conference Games Won" dataDxfId="4"/>
     <tableColumn id="32" xr3:uid="{9BBF7A55-6F8A-3B46-9E03-6BA3A4EAB1F9}" name="Conference Games Lost" dataDxfId="3"/>
-    <tableColumn id="33" xr3:uid="{FC84F4F9-44DC-114D-9E12-D98A830046E9}" name="Minutes" dataDxfId="2"/>
-    <tableColumn id="34" xr3:uid="{6D9FE05C-B8EE-594C-8F4F-8E8EEE4D2494}" name="AP Poll Ranking" dataDxfId="1"/>
-    <tableColumn id="35" xr3:uid="{151192C7-A29B-0C49-8873-EC3BD91274CF}" name="USA Today Coaches Poll Ranking" dataDxfId="0"/>
+    <tableColumn id="33" xr3:uid="{FC84F4F9-44DC-114D-9E12-D98A830046E9}" name="Minutes" dataDxfId="0"/>
+    <tableColumn id="34" xr3:uid="{6D9FE05C-B8EE-594C-8F4F-8E8EEE4D2494}" name="AP Poll Ranking" dataDxfId="2"/>
+    <tableColumn id="35" xr3:uid="{151192C7-A29B-0C49-8873-EC3BD91274CF}" name="USA Today Coaches Poll Ranking" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -825,7 +822,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD2AB4CB-49C7-5748-9B5D-D1933262EFEF}">
   <dimension ref="A1:AI45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="AB24" workbookViewId="0">
+      <selection activeCell="AG36" sqref="AG36"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4708,9 +4707,6 @@
       <c r="AF36" s="2">
         <v>3</v>
       </c>
-      <c r="AG36" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="AH36" s="2">
         <v>13</v>
       </c>
@@ -4815,9 +4811,6 @@
       <c r="AF37" s="2">
         <v>13</v>
       </c>
-      <c r="AG37" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="AH37" s="5" t="s">
         <v>38</v>
       </c>
@@ -4827,7 +4820,7 @@
     </row>
     <row r="38" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>36</v>
@@ -4921,9 +4914,6 @@
       </c>
       <c r="AF38" s="2">
         <v>2</v>
-      </c>
-      <c r="AG38" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="AH38" s="2">
         <v>4</v>
@@ -4934,7 +4924,7 @@
     </row>
     <row r="39" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>37</v>
@@ -5028,9 +5018,6 @@
       </c>
       <c r="AF39" s="2">
         <v>14</v>
-      </c>
-      <c r="AG39" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="AH39" s="5" t="s">
         <v>38</v>
@@ -5041,7 +5028,7 @@
     </row>
     <row r="40" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>36</v>
@@ -5135,9 +5122,6 @@
       </c>
       <c r="AF40" s="2">
         <v>1</v>
-      </c>
-      <c r="AG40" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="AH40" s="2">
         <v>5</v>
@@ -5148,7 +5132,7 @@
     </row>
     <row r="41" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>37</v>
@@ -5242,9 +5226,6 @@
       </c>
       <c r="AF41" s="2">
         <v>15</v>
-      </c>
-      <c r="AG41" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="AH41" s="5" t="s">
         <v>38</v>
@@ -5255,7 +5236,7 @@
     </row>
     <row r="42" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>36</v>
@@ -5349,9 +5330,6 @@
       </c>
       <c r="AF42" s="2">
         <v>6</v>
-      </c>
-      <c r="AG42" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="AH42" s="2">
         <v>14</v>
@@ -5362,7 +5340,7 @@
     </row>
     <row r="43" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>37</v>
@@ -5456,9 +5434,6 @@
       </c>
       <c r="AF43" s="2">
         <v>10</v>
-      </c>
-      <c r="AG43" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="AH43" s="5" t="s">
         <v>38</v>
@@ -5469,7 +5444,7 @@
     </row>
     <row r="44" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>36</v>
@@ -5563,9 +5538,6 @@
       </c>
       <c r="AF44" s="2">
         <v>9</v>
-      </c>
-      <c r="AG44" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="AH44" s="2" t="s">
         <v>40</v>
@@ -5576,7 +5548,7 @@
     </row>
     <row r="45" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>37</v>
@@ -5670,9 +5642,6 @@
       </c>
       <c r="AF45" s="2">
         <v>7</v>
-      </c>
-      <c r="AG45" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="AH45" s="2" t="s">
         <v>38</v>
@@ -5705,60 +5674,60 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>62</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B2" t="s">
         <v>64</v>
-      </c>
-      <c r="B2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" t="s">
         <v>66</v>
-      </c>
-      <c r="B3" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
         <v>68</v>
-      </c>
-      <c r="B4" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B5" t="s">
         <v>70</v>
-      </c>
-      <c r="B5" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>72</v>
+      </c>
+      <c r="B7" t="s">
         <v>73</v>
-      </c>
-      <c r="B7" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>